<commit_message>
:soap: change sheets name
</commit_message>
<xml_diff>
--- a/task1/bisection.xlsx
+++ b/task1/bisection.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn\metnum-uwu\task1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FE1D08-9B56-4121-9B22-61D0F3A696A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5534A85C-807C-4216-A609-087429AC2A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bisection" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -193,9 +193,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -214,12 +211,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -227,6 +218,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -517,759 +517,759 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5"/>
-    <col min="2" max="3" width="13.77734375" style="5" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="5"/>
-    <col min="6" max="6" width="10.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="8.21875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="9.21875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="13.21875" style="5" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="3" width="13.77734375" style="4" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="4"/>
+    <col min="6" max="6" width="10.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="8.21875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9.21875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="13.21875" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>-4.2300000000000004</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>1</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="8">
         <v>2</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <f>(G6+H6)/2</f>
         <v>1.5</v>
       </c>
-      <c r="J6" s="2">
-        <f>2.05*(G6^3)-1.12*(G6^3)-4.23</f>
+      <c r="J6" s="1">
+        <f t="shared" ref="J6:L7" si="0">2.05*(G6^3)-1.12*(G6^3)-4.23</f>
         <v>-3.3000000000000007</v>
       </c>
-      <c r="K6" s="2">
-        <f>2.05*(H6^3)-1.12*(H6^3)-4.23</f>
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
         <v>3.2099999999999973</v>
       </c>
-      <c r="L6" s="2">
-        <f>2.05*(I6^3)-1.12*(I6^3)-4.23</f>
+      <c r="L6" s="1">
+        <f t="shared" si="0"/>
         <v>-1.0912500000000014</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <f>J6*L6</f>
         <v>3.6011250000000055</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <f>ABS(L6)</f>
         <v>1.0912500000000014</v>
       </c>
-      <c r="O6" s="2" t="str">
+      <c r="O6" s="1" t="str">
         <f>IF(N6&lt;0.0001, "STOP", "CONTINUE")</f>
         <v>CONTINUE</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="8">
         <v>1</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>-3.3</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f>IF(M6&gt;0,I6,G6)</f>
         <v>1.5</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <f>IF(M6&lt;0,I6,H6)</f>
         <v>2</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f>(G7+H7)/2</f>
         <v>1.75</v>
       </c>
-      <c r="J7" s="2">
-        <f>2.05*(G7^3)-1.12*(G7^3)-4.23</f>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
         <v>-1.0912500000000014</v>
       </c>
-      <c r="K7" s="2">
-        <f>2.05*(H7^3)-1.12*(H7^3)-4.23</f>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
         <v>3.2099999999999973</v>
       </c>
-      <c r="L7" s="2">
-        <f>2.05*(I7^3)-1.12*(I7^3)-4.23</f>
+      <c r="L7" s="1">
+        <f t="shared" si="0"/>
         <v>0.75421874999999883</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="1">
         <f>J7*L7</f>
         <v>-0.82304121093749971</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="1">
         <f>ABS(L7)</f>
         <v>0.75421874999999883</v>
       </c>
-      <c r="O7" s="2" t="str">
+      <c r="O7" s="1" t="str">
         <f>IF(N7&lt;0.0001, "STOP", "CONTINUE")</f>
         <v>CONTINUE</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="8">
         <v>2</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>3.21</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>3</v>
       </c>
-      <c r="G8" s="2">
-        <f t="shared" ref="G8:G20" si="0">IF(M7&gt;0,I7,G7)</f>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G20" si="1">IF(M7&gt;0,I7,G7)</f>
         <v>1.5</v>
       </c>
-      <c r="H8" s="2">
-        <f t="shared" ref="H8:H20" si="1">IF(M7&lt;0,I7,H7)</f>
+      <c r="H8" s="1">
+        <f t="shared" ref="H8:H20" si="2">IF(M7&lt;0,I7,H7)</f>
         <v>1.75</v>
       </c>
-      <c r="I8" s="2">
-        <f t="shared" ref="I8:I20" si="2">(G8+H8)/2</f>
+      <c r="I8" s="1">
+        <f t="shared" ref="I8:I20" si="3">(G8+H8)/2</f>
         <v>1.625</v>
       </c>
-      <c r="J8" s="2">
-        <f t="shared" ref="J8:J20" si="3">2.05*(G8^3)-1.12*(G8^3)-4.23</f>
+      <c r="J8" s="1">
+        <f t="shared" ref="J8:J20" si="4">2.05*(G8^3)-1.12*(G8^3)-4.23</f>
         <v>-1.0912500000000014</v>
       </c>
-      <c r="K8" s="2">
-        <f t="shared" ref="K8:K20" si="4">2.05*(H8^3)-1.12*(H8^3)-4.23</f>
+      <c r="K8" s="1">
+        <f t="shared" ref="K8:K20" si="5">2.05*(H8^3)-1.12*(H8^3)-4.23</f>
         <v>0.75421874999999883</v>
       </c>
-      <c r="L8" s="2">
-        <f t="shared" ref="L8:L20" si="5">2.05*(I8^3)-1.12*(I8^3)-4.23</f>
+      <c r="L8" s="1">
+        <f t="shared" ref="L8:L20" si="6">2.05*(I8^3)-1.12*(I8^3)-4.23</f>
         <v>-0.23935546875000213</v>
       </c>
-      <c r="M8" s="2">
-        <f t="shared" ref="M8:M20" si="6">J8*L8</f>
+      <c r="M8" s="1">
+        <f t="shared" ref="M8:M20" si="7">J8*L8</f>
         <v>0.26119665527344016</v>
       </c>
-      <c r="N8" s="2">
-        <f t="shared" ref="N8:N20" si="7">ABS(L8)</f>
+      <c r="N8" s="1">
+        <f t="shared" ref="N8:N20" si="8">ABS(L8)</f>
         <v>0.23935546875000213</v>
       </c>
-      <c r="O8" s="2" t="str">
-        <f t="shared" ref="O8:O20" si="8">IF(N8&lt;0.0001, "STOP", "CONTINUE")</f>
+      <c r="O8" s="1" t="str">
+        <f t="shared" ref="O8:O20" si="9">IF(N8&lt;0.0001, "STOP", "CONTINUE")</f>
         <v>CONTINUE</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>20.88</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>4</v>
       </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
         <v>1.625</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>1.75</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="3"/>
+        <v>1.6875</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.23935546875000213</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="5"/>
+        <v>0.75421874999999883</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="6"/>
+        <v>0.23904052734374748</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="7"/>
+        <v>-5.7215657472610378E-2</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="8"/>
+        <v>0.23904052734374748</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>55.29</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>1.75</v>
-      </c>
-      <c r="I9" s="2">
+        <v>1.625</v>
+      </c>
+      <c r="H10" s="1">
         <f t="shared" si="2"/>
         <v>1.6875</v>
       </c>
-      <c r="J9" s="2">
+      <c r="I10" s="1">
         <f t="shared" si="3"/>
+        <v>1.65625</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="4"/>
         <v>-0.23935546875000213</v>
       </c>
-      <c r="K9" s="2">
-        <f t="shared" si="4"/>
-        <v>0.75421874999999883</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="K10" s="1">
         <f t="shared" si="5"/>
         <v>0.23904052734374748</v>
       </c>
-      <c r="M9" s="2">
+      <c r="L10" s="1">
         <f t="shared" si="6"/>
-        <v>-5.7215657472610378E-2</v>
-      </c>
-      <c r="N9" s="2">
+        <v>-4.6701049804704908E-3</v>
+      </c>
+      <c r="M10" s="1">
         <f t="shared" si="7"/>
+        <v>1.1178151667122339E-3</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="8"/>
+        <v>4.6701049804704908E-3</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>112.02</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.65625</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>1.6875</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="3"/>
+        <v>1.671875</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="4"/>
+        <v>-4.6701049804704908E-3</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="5"/>
         <v>0.23904052734374748</v>
       </c>
-      <c r="O9" s="2" t="str">
+      <c r="L11" s="1">
+        <f t="shared" si="6"/>
+        <v>0.11604640960693224</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="7"/>
+        <v>-5.4194891547105291E-4</v>
+      </c>
+      <c r="N11" s="1">
         <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2">
-        <v>55.29</v>
-      </c>
-      <c r="F10" s="2">
-        <v>5</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>1.625</v>
-      </c>
-      <c r="H10" s="2">
+        <v>0.11604640960693224</v>
+      </c>
+      <c r="O11" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>196.65</v>
+      </c>
+      <c r="F12" s="1">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>1.6875</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="2"/>
         <v>1.65625</v>
       </c>
-      <c r="J10" s="2">
-        <f t="shared" si="3"/>
-        <v>-0.23935546875000213</v>
-      </c>
-      <c r="K10" s="2">
-        <f t="shared" si="4"/>
-        <v>0.23904052734374748</v>
-      </c>
-      <c r="L10" s="2">
-        <f t="shared" si="5"/>
-        <v>-4.6701049804704908E-3</v>
-      </c>
-      <c r="M10" s="2">
-        <f t="shared" si="6"/>
-        <v>1.1178151667122339E-3</v>
-      </c>
-      <c r="N10" s="2">
-        <f t="shared" si="7"/>
-        <v>4.6701049804704908E-3</v>
-      </c>
-      <c r="O10" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2">
-        <v>112.02</v>
-      </c>
-      <c r="F11" s="2">
-        <v>6</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>1.65625</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6875</v>
-      </c>
-      <c r="I11" s="2">
+      <c r="H12" s="1">
         <f t="shared" si="2"/>
         <v>1.671875</v>
       </c>
-      <c r="J11" s="2">
+      <c r="I12" s="1">
         <f t="shared" si="3"/>
+        <v>1.6640625</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="4"/>
         <v>-4.6701049804704908E-3</v>
       </c>
-      <c r="K11" s="2">
-        <f t="shared" si="4"/>
-        <v>0.23904052734374748</v>
-      </c>
-      <c r="L11" s="2">
+      <c r="K12" s="1">
         <f t="shared" si="5"/>
         <v>0.11604640960693224</v>
       </c>
-      <c r="M11" s="2">
+      <c r="L12" s="1">
         <f t="shared" si="6"/>
-        <v>-5.4194891547105291E-4</v>
-      </c>
-      <c r="N11" s="2">
+        <v>5.5404782295225274E-2</v>
+      </c>
+      <c r="M12" s="1">
         <f t="shared" si="7"/>
-        <v>0.11604640960693224</v>
-      </c>
-      <c r="O11" s="2" t="str">
+        <v>-2.5874614973881485E-4</v>
+      </c>
+      <c r="N12" s="1">
         <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2">
-        <v>196.65</v>
-      </c>
-      <c r="F12" s="2">
+        <v>5.5404782295225274E-2</v>
+      </c>
+      <c r="O12" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
         <v>7</v>
       </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
+      <c r="C13" s="1">
+        <v>314.76</v>
+      </c>
+      <c r="F13" s="1">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
         <v>1.65625</v>
       </c>
-      <c r="H12" s="2">
-        <f t="shared" si="1"/>
-        <v>1.671875</v>
-      </c>
-      <c r="I12" s="2">
+      <c r="H13" s="1">
         <f t="shared" si="2"/>
         <v>1.6640625</v>
       </c>
-      <c r="J12" s="2">
+      <c r="I13" s="1">
         <f t="shared" si="3"/>
+        <v>1.66015625</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="4"/>
         <v>-4.6701049804704908E-3</v>
       </c>
-      <c r="K12" s="2">
-        <f t="shared" si="4"/>
-        <v>0.11604640960693224</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="K13" s="1">
         <f t="shared" si="5"/>
         <v>5.5404782295225274E-2</v>
       </c>
-      <c r="M12" s="2">
+      <c r="L13" s="1">
         <f t="shared" si="6"/>
-        <v>-2.5874614973881485E-4</v>
-      </c>
-      <c r="N12" s="2">
+        <v>2.5296662449835416E-2</v>
+      </c>
+      <c r="M13" s="1">
         <f t="shared" si="7"/>
-        <v>5.5404782295225274E-2</v>
-      </c>
-      <c r="O12" s="2" t="str">
+        <v>-1.1813806929625722E-4</v>
+      </c>
+      <c r="N13" s="1">
         <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2">
-        <v>314.76</v>
-      </c>
-      <c r="F13" s="2">
+        <v>2.5296662449835416E-2</v>
+      </c>
+      <c r="O13" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
         <v>8</v>
       </c>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
+      <c r="C14" s="1">
+        <v>471.93</v>
+      </c>
+      <c r="F14" s="1">
+        <v>9</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
         <v>1.65625</v>
       </c>
-      <c r="H13" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6640625</v>
-      </c>
-      <c r="I13" s="2">
+      <c r="H14" s="1">
         <f t="shared" si="2"/>
         <v>1.66015625</v>
       </c>
-      <c r="J13" s="2">
+      <c r="I14" s="1">
         <f t="shared" si="3"/>
+        <v>1.658203125</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="4"/>
         <v>-4.6701049804704908E-3</v>
       </c>
-      <c r="K13" s="2">
-        <f t="shared" si="4"/>
-        <v>5.5404782295225274E-2</v>
-      </c>
-      <c r="L13" s="2">
+      <c r="K14" s="1">
         <f t="shared" si="5"/>
         <v>2.5296662449835416E-2</v>
       </c>
-      <c r="M13" s="2">
+      <c r="L14" s="1">
         <f t="shared" si="6"/>
-        <v>-1.1813806929625722E-4</v>
-      </c>
-      <c r="N13" s="2">
+        <v>1.0295630469915551E-2</v>
+      </c>
+      <c r="M14" s="1">
         <f t="shared" si="7"/>
-        <v>2.5296662449835416E-2</v>
-      </c>
-      <c r="O13" s="2" t="str">
+        <v>-4.8081675134636357E-5</v>
+      </c>
+      <c r="N14" s="1">
         <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2">
-        <v>471.93</v>
-      </c>
-      <c r="F14" s="2">
+        <v>1.0295630469915551E-2</v>
+      </c>
+      <c r="O14" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
         <v>9</v>
       </c>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
+      <c r="C15" s="1">
+        <v>673.74</v>
+      </c>
+      <c r="F15" s="1">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="1"/>
         <v>1.65625</v>
       </c>
-      <c r="H14" s="2">
-        <f t="shared" si="1"/>
-        <v>1.66015625</v>
-      </c>
-      <c r="I14" s="2">
+      <c r="H15" s="1">
         <f t="shared" si="2"/>
         <v>1.658203125</v>
       </c>
-      <c r="J14" s="2">
+      <c r="I15" s="1">
         <f t="shared" si="3"/>
+        <v>1.6572265625</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="4"/>
         <v>-4.6701049804704908E-3</v>
       </c>
-      <c r="K14" s="2">
-        <f t="shared" si="4"/>
-        <v>2.5296662449835416E-2</v>
-      </c>
-      <c r="L14" s="2">
+      <c r="K15" s="1">
         <f t="shared" si="5"/>
         <v>1.0295630469915551E-2</v>
       </c>
-      <c r="M14" s="2">
+      <c r="L15" s="1">
         <f t="shared" si="6"/>
-        <v>-4.8081675134636357E-5</v>
-      </c>
-      <c r="N14" s="2">
+        <v>2.8083532769223041E-3</v>
+      </c>
+      <c r="M15" s="1">
         <f t="shared" si="7"/>
-        <v>1.0295630469915551E-2</v>
-      </c>
-      <c r="O14" s="2" t="str">
+        <v>-1.3115304625475477E-5</v>
+      </c>
+      <c r="N15" s="1">
         <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2">
-        <v>673.74</v>
-      </c>
-      <c r="F15" s="2">
+        <v>2.8083532769223041E-3</v>
+      </c>
+      <c r="O15" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
         <v>10</v>
       </c>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
+      <c r="C16" s="1">
+        <v>925.77</v>
+      </c>
+      <c r="F16" s="1">
+        <v>11</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
         <v>1.65625</v>
       </c>
-      <c r="H15" s="2">
-        <f t="shared" si="1"/>
-        <v>1.658203125</v>
-      </c>
-      <c r="I15" s="2">
+      <c r="H16" s="1">
         <f t="shared" si="2"/>
         <v>1.6572265625</v>
       </c>
-      <c r="J15" s="2">
+      <c r="I16" s="1">
         <f t="shared" si="3"/>
+        <v>1.65673828125</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="4"/>
         <v>-4.6701049804704908E-3</v>
       </c>
-      <c r="K15" s="2">
-        <f t="shared" si="4"/>
-        <v>1.0295630469915551E-2</v>
-      </c>
-      <c r="L15" s="2">
+      <c r="K16" s="1">
         <f t="shared" si="5"/>
         <v>2.8083532769223041E-3</v>
       </c>
-      <c r="M15" s="2">
+      <c r="L16" s="1">
         <f t="shared" si="6"/>
-        <v>-1.3115304625475477E-5</v>
-      </c>
-      <c r="N15" s="2">
+        <v>-9.319778939262946E-4</v>
+      </c>
+      <c r="M16" s="1">
         <f t="shared" si="7"/>
+        <v>4.3524346041135869E-6</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="8"/>
+        <v>9.319778939262946E-4</v>
+      </c>
+      <c r="O16" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F17" s="1">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.65673828125</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.6572265625</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="3"/>
+        <v>1.656982421875</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="4"/>
+        <v>-9.319778939262946E-4</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="5"/>
         <v>2.8083532769223041E-3</v>
       </c>
-      <c r="O15" s="2" t="str">
+      <c r="L17" s="1">
+        <f t="shared" si="6"/>
+        <v>9.3791214035920945E-4</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="7"/>
+        <v>-8.741133812598792E-7</v>
+      </c>
+      <c r="N17" s="1">
         <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
-        <v>10</v>
-      </c>
-      <c r="C16" s="2">
-        <v>925.77</v>
-      </c>
-      <c r="F16" s="2">
-        <v>11</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>1.65625</v>
-      </c>
-      <c r="H16" s="2">
+        <v>9.3791214035920945E-4</v>
+      </c>
+      <c r="O17" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f>_xlfn.CONCAT(" ", 10^-4)</f>
+        <v xml:space="preserve"> 0,0001</v>
+      </c>
+      <c r="F18" s="9">
+        <v>13</v>
+      </c>
+      <c r="G18" s="9">
         <f t="shared" si="1"/>
-        <v>1.6572265625</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" si="2"/>
         <v>1.65673828125</v>
       </c>
-      <c r="J16" s="2">
-        <f t="shared" si="3"/>
-        <v>-4.6701049804704908E-3</v>
-      </c>
-      <c r="K16" s="2">
-        <f t="shared" si="4"/>
-        <v>2.8083532769223041E-3</v>
-      </c>
-      <c r="L16" s="2">
-        <f t="shared" si="5"/>
-        <v>-9.319778939262946E-4</v>
-      </c>
-      <c r="M16" s="2">
-        <f t="shared" si="6"/>
-        <v>4.3524346041135869E-6</v>
-      </c>
-      <c r="N16" s="2">
-        <f t="shared" si="7"/>
-        <v>9.319778939262946E-4</v>
-      </c>
-      <c r="O16" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F17" s="2">
-        <v>12</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>1.65673828125</v>
-      </c>
-      <c r="H17" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6572265625</v>
-      </c>
-      <c r="I17" s="2">
+      <c r="H18" s="9">
         <f t="shared" si="2"/>
         <v>1.656982421875</v>
       </c>
-      <c r="J17" s="2">
+      <c r="I18" s="9">
         <f t="shared" si="3"/>
+        <v>1.6568603515625</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" si="4"/>
         <v>-9.319778939262946E-4</v>
       </c>
-      <c r="K17" s="2">
-        <f t="shared" si="4"/>
-        <v>2.8083532769223041E-3</v>
-      </c>
-      <c r="L17" s="2">
+      <c r="K18" s="9">
         <f t="shared" si="5"/>
         <v>9.3791214035920945E-4</v>
       </c>
-      <c r="M17" s="2">
+      <c r="L18" s="9">
         <f t="shared" si="6"/>
-        <v>-8.741133812598792E-7</v>
-      </c>
-      <c r="N17" s="2">
+        <v>2.8982405080313356E-6</v>
+      </c>
+      <c r="M18" s="9">
         <f t="shared" si="7"/>
-        <v>9.3791214035920945E-4</v>
-      </c>
-      <c r="O17" s="2" t="str">
+        <v>-2.7010960847669182E-9</v>
+      </c>
+      <c r="N18" s="9">
         <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="6" t="str">
-        <f>_xlfn.CONCAT(" ", 10^-4)</f>
-        <v xml:space="preserve"> 0,0001</v>
-      </c>
-      <c r="F18" s="12">
-        <v>13</v>
-      </c>
-      <c r="G18" s="12">
-        <f t="shared" si="0"/>
+        <v>2.8982405080313356E-6</v>
+      </c>
+      <c r="O18" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v>STOP</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F19" s="1">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
         <v>1.65673828125</v>
       </c>
-      <c r="H18" s="12">
-        <f t="shared" si="1"/>
-        <v>1.656982421875</v>
-      </c>
-      <c r="I18" s="12">
+      <c r="H19" s="1">
         <f t="shared" si="2"/>
         <v>1.6568603515625</v>
       </c>
-      <c r="J18" s="12">
+      <c r="I19" s="1">
         <f t="shared" si="3"/>
+        <v>1.65679931640625</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="4"/>
         <v>-9.319778939262946E-4</v>
       </c>
-      <c r="K18" s="12">
-        <f t="shared" si="4"/>
-        <v>9.3791214035920945E-4</v>
-      </c>
-      <c r="L18" s="12">
+      <c r="K19" s="1">
         <f t="shared" si="5"/>
         <v>2.8982405080313356E-6</v>
       </c>
-      <c r="M18" s="12">
+      <c r="L19" s="1">
         <f t="shared" si="6"/>
-        <v>-2.7010960847669182E-9</v>
-      </c>
-      <c r="N18" s="12">
+        <v>-4.6455704675185672E-4</v>
+      </c>
+      <c r="M19" s="1">
         <f t="shared" si="7"/>
+        <v>4.3295689804041459E-7</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="8"/>
+        <v>4.6455704675185672E-4</v>
+      </c>
+      <c r="O19" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F20" s="1">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.65679931640625</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>1.6568603515625</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="3"/>
+        <v>1.656829833984375</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="4"/>
+        <v>-4.6455704675185672E-4</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="5"/>
         <v>2.8982405080313356E-6</v>
       </c>
-      <c r="O18" s="12" t="str">
+      <c r="L20" s="1">
+        <f t="shared" si="6"/>
+        <v>-2.3083370821286309E-4</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="7"/>
+        <v>1.0723542577814749E-7</v>
+      </c>
+      <c r="N20" s="1">
         <f t="shared" si="8"/>
-        <v>STOP</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F19" s="2">
-        <v>14</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>1.65673828125</v>
-      </c>
-      <c r="H19" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6568603515625</v>
-      </c>
-      <c r="I19" s="2">
-        <f t="shared" si="2"/>
-        <v>1.65679931640625</v>
-      </c>
-      <c r="J19" s="2">
-        <f t="shared" si="3"/>
-        <v>-9.319778939262946E-4</v>
-      </c>
-      <c r="K19" s="2">
-        <f t="shared" si="4"/>
-        <v>2.8982405080313356E-6</v>
-      </c>
-      <c r="L19" s="2">
-        <f t="shared" si="5"/>
-        <v>-4.6455704675185672E-4</v>
-      </c>
-      <c r="M19" s="2">
-        <f t="shared" si="6"/>
-        <v>4.3295689804041459E-7</v>
-      </c>
-      <c r="N19" s="2">
-        <f t="shared" si="7"/>
-        <v>4.6455704675185672E-4</v>
-      </c>
-      <c r="O19" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>CONTINUE</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F20" s="2">
-        <v>15</v>
-      </c>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>1.65679931640625</v>
-      </c>
-      <c r="H20" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6568603515625</v>
-      </c>
-      <c r="I20" s="2">
-        <f t="shared" si="2"/>
-        <v>1.656829833984375</v>
-      </c>
-      <c r="J20" s="2">
-        <f t="shared" si="3"/>
-        <v>-4.6455704675185672E-4</v>
-      </c>
-      <c r="K20" s="2">
-        <f t="shared" si="4"/>
-        <v>2.8982405080313356E-6</v>
-      </c>
-      <c r="L20" s="2">
-        <f t="shared" si="5"/>
-        <v>-2.3083370821286309E-4</v>
-      </c>
-      <c r="M20" s="2">
-        <f t="shared" si="6"/>
-        <v>1.0723542577814749E-7</v>
-      </c>
-      <c r="N20" s="2">
-        <f t="shared" si="7"/>
         <v>2.3083370821286309E-4</v>
       </c>
-      <c r="O20" s="2" t="str">
-        <f t="shared" si="8"/>
+      <c r="O20" s="1" t="str">
+        <f t="shared" si="9"/>
         <v>CONTINUE</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:memo: change equation formula
</commit_message>
<xml_diff>
--- a/task1/bisection.xlsx
+++ b/task1/bisection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn\metnum-uwu\task1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5534A85C-807C-4216-A609-087429AC2A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F5E375-032A-4AE2-A62C-BB842435027F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>f(x) = 2.05x^3-1.12x^3-4.23</t>
-  </si>
   <si>
     <t>X</t>
   </si>
@@ -82,6 +79,9 @@
   <si>
     <t>Status</t>
   </si>
+  <si>
+    <t>f(x) = 2.99x^5-1.12x^3-1.26</t>
+  </si>
 </sst>
 </file>
 
@@ -109,7 +109,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,7 +148,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -191,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -217,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -227,6 +233,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -509,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:O20"/>
+  <dimension ref="A3:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C3"/>
@@ -535,7 +547,7 @@
   <sheetData>
     <row r="3" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C3" s="11"/>
     </row>
@@ -545,81 +557,82 @@
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="C6" s="1">
-        <v>-4.2300000000000004</v>
+        <f>2.99*(B6^5)-1.12*(B6^3)-1.26</f>
+        <v>-9205.01</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
         <v>1</v>
-      </c>
-      <c r="H6" s="8">
-        <v>2</v>
       </c>
       <c r="I6" s="1">
         <f>(G6+H6)/2</f>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" ref="J6:L7" si="0">2.05*(G6^3)-1.12*(G6^3)-4.23</f>
-        <v>-3.3000000000000007</v>
+        <f>2.99*(G6^5)-1.12*(G6^3)-1.26</f>
+        <v>-1.26</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="0"/>
-        <v>3.2099999999999973</v>
+        <f>2.99*(H6^5)-1.12*(H6^3)-1.26</f>
+        <v>0.6100000000000001</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="0"/>
-        <v>-1.0912500000000014</v>
+        <f>2.99*(I6^5)-1.12*(I6^3)-1.26</f>
+        <v>-1.3065625000000001</v>
       </c>
       <c r="M6" s="1">
         <f>J6*L6</f>
-        <v>3.6011250000000055</v>
+        <v>1.6462687500000002</v>
       </c>
       <c r="N6" s="1">
         <f>ABS(L6)</f>
-        <v>1.0912500000000014</v>
+        <v>1.3065625000000001</v>
       </c>
       <c r="O6" s="1" t="str">
         <f>IF(N6&lt;0.0001, "STOP", "CONTINUE")</f>
@@ -627,49 +640,47 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>-3.3</v>
+      <c r="B7" s="9">
+        <v>-4</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" ref="C7:C16" si="0">2.99*(B7^5)-1.12*(B7^3)-1.26</f>
+        <v>-2991.3400000000006</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
       </c>
       <c r="G7" s="1">
         <f>IF(M6&gt;0,I6,G6)</f>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="1">
         <f>IF(M6&lt;0,I6,H6)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
-        <f>(G7+H7)/2</f>
-        <v>1.75</v>
+        <f t="shared" ref="I7:I25" si="1">(G7+H7)/2</f>
+        <v>0.75</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="0"/>
-        <v>-1.0912500000000014</v>
+        <f t="shared" ref="J7:J25" si="2">2.99*(G7^5)-1.12*(G7^3)-1.26</f>
+        <v>-1.3065625000000001</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="0"/>
-        <v>3.2099999999999973</v>
+        <f t="shared" ref="K7:K25" si="3">2.99*(H7^5)-1.12*(H7^3)-1.26</f>
+        <v>0.6100000000000001</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.75421874999999883</v>
+        <f t="shared" ref="L7:L25" si="4">2.99*(I7^5)-1.12*(I7^3)-1.26</f>
+        <v>-1.022958984375</v>
       </c>
       <c r="M7" s="1">
-        <f>J7*L7</f>
-        <v>-0.82304121093749971</v>
+        <f t="shared" ref="M7:M25" si="5">J7*L7</f>
+        <v>1.336559848022461</v>
       </c>
       <c r="N7" s="1">
-        <f>ABS(L7)</f>
-        <v>0.75421874999999883</v>
+        <f t="shared" ref="N7:N25" si="6">ABS(L7)</f>
+        <v>1.022958984375</v>
       </c>
       <c r="O7" s="1" t="str">
         <f>IF(N7&lt;0.0001, "STOP", "CONTINUE")</f>
@@ -677,96 +688,95 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="8">
-        <v>2</v>
-      </c>
-      <c r="C8" s="8">
-        <v>3.21</v>
+      <c r="B8" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>-697.59</v>
       </c>
       <c r="F8" s="1">
         <v>3</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G20" si="1">IF(M7&gt;0,I7,G7)</f>
-        <v>1.5</v>
+        <f t="shared" ref="G8:G20" si="7">IF(M7&gt;0,I7,G7)</f>
+        <v>0.75</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8:H20" si="2">IF(M7&lt;0,I7,H7)</f>
-        <v>1.75</v>
+        <f t="shared" ref="H8:H20" si="8">IF(M7&lt;0,I7,H7)</f>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ref="I8:I20" si="3">(G8+H8)/2</f>
-        <v>1.625</v>
+        <f t="shared" si="1"/>
+        <v>0.875</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" ref="J8:J20" si="4">2.05*(G8^3)-1.12*(G8^3)-4.23</f>
-        <v>-1.0912500000000014</v>
+        <f t="shared" si="2"/>
+        <v>-1.022958984375</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" ref="K8:K20" si="5">2.05*(H8^3)-1.12*(H8^3)-4.23</f>
-        <v>0.75421874999999883</v>
+        <f t="shared" si="3"/>
+        <v>0.6100000000000001</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" ref="L8:L20" si="6">2.05*(I8^3)-1.12*(I8^3)-4.23</f>
-        <v>-0.23935546875000213</v>
+        <f t="shared" si="4"/>
+        <v>-0.4767147827148438</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" ref="M8:M20" si="7">J8*L8</f>
-        <v>0.26119665527344016</v>
+        <f t="shared" si="5"/>
+        <v>0.48765966996252541</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" ref="N8:N20" si="8">ABS(L8)</f>
-        <v>0.23935546875000213</v>
+        <f t="shared" si="6"/>
+        <v>0.4767147827148438</v>
       </c>
       <c r="O8" s="1" t="str">
-        <f t="shared" ref="O8:O20" si="9">IF(N8&lt;0.0001, "STOP", "CONTINUE")</f>
+        <f t="shared" ref="O8:O25" si="9">IF(N8&lt;0.0001, "STOP", "CONTINUE")</f>
         <v>CONTINUE</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
-        <v>3</v>
+      <c r="B9" s="9">
+        <v>-2</v>
       </c>
       <c r="C9" s="1">
-        <v>20.88</v>
+        <f t="shared" si="0"/>
+        <v>-87.98</v>
       </c>
       <c r="F9" s="1">
         <v>4</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="1"/>
-        <v>1.625</v>
+        <f t="shared" si="7"/>
+        <v>0.875</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="2"/>
-        <v>1.75</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="3"/>
-        <v>1.6875</v>
+        <f t="shared" si="1"/>
+        <v>0.9375</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="4"/>
-        <v>-0.23935546875000213</v>
+        <f t="shared" si="2"/>
+        <v>-0.4767147827148438</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="5"/>
-        <v>0.75421874999999883</v>
+        <f t="shared" si="3"/>
+        <v>0.6100000000000001</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="6"/>
-        <v>0.23904052734374748</v>
+        <f t="shared" si="4"/>
+        <v>-1.7504224777221689E-2</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="7"/>
-        <v>-5.7215657472610378E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.3445227112650226E-3</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="8"/>
-        <v>0.23904052734374748</v>
+        <f t="shared" si="6"/>
+        <v>1.7504224777221689E-2</v>
       </c>
       <c r="O9" s="1" t="str">
         <f t="shared" si="9"/>
@@ -774,46 +784,47 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
-        <v>4</v>
+      <c r="B10" s="9">
+        <v>-1</v>
       </c>
       <c r="C10" s="1">
-        <v>55.29</v>
+        <f t="shared" si="0"/>
+        <v>-3.13</v>
       </c>
       <c r="F10" s="1">
         <v>5</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>1.625</v>
+        <f t="shared" si="7"/>
+        <v>0.9375</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6875</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="3"/>
-        <v>1.65625</v>
+        <f t="shared" si="1"/>
+        <v>0.96875</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="4"/>
-        <v>-0.23935546875000213</v>
+        <f t="shared" si="2"/>
+        <v>-1.7504224777221689E-2</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="5"/>
-        <v>0.23904052734374748</v>
+        <f t="shared" si="3"/>
+        <v>0.6100000000000001</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="6"/>
-        <v>-4.6701049804704908E-3</v>
+        <f t="shared" si="4"/>
+        <v>0.27286634117364894</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" si="7"/>
-        <v>1.1178151667122339E-3</v>
+        <f t="shared" si="5"/>
+        <v>-4.776313770041612E-3</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="8"/>
-        <v>4.6701049804704908E-3</v>
+        <f t="shared" si="6"/>
+        <v>0.27286634117364894</v>
       </c>
       <c r="O10" s="1" t="str">
         <f t="shared" si="9"/>
@@ -821,46 +832,50 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="1">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
-        <v>112.02</v>
+      <c r="B11" s="13">
+        <v>0</v>
+      </c>
+      <c r="C11" s="13">
+        <f t="shared" si="0"/>
+        <v>-1.26</v>
       </c>
       <c r="F11" s="1">
         <v>6</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>1.65625</v>
+        <f t="shared" si="7"/>
+        <v>0.9375</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6875</v>
+        <f t="shared" si="8"/>
+        <v>0.96875</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="3"/>
-        <v>1.671875</v>
+        <f t="shared" si="1"/>
+        <v>0.953125</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="4"/>
-        <v>-4.6701049804704908E-3</v>
+        <f t="shared" si="2"/>
+        <v>-1.7504224777221689E-2</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="5"/>
-        <v>0.23904052734374748</v>
+        <f t="shared" si="3"/>
+        <v>0.27286634117364894</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="6"/>
-        <v>0.11604640960693224</v>
+        <f t="shared" si="4"/>
+        <v>0.12214143260382126</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="7"/>
-        <v>-5.4194891547105291E-4</v>
+        <f t="shared" si="5"/>
+        <v>-2.1379910909091614E-3</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="8"/>
-        <v>0.11604640960693224</v>
+        <f t="shared" si="6"/>
+        <v>0.12214143260382126</v>
       </c>
       <c r="O11" s="1" t="str">
         <f t="shared" si="9"/>
@@ -868,46 +883,50 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="1">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1">
-        <v>196.65</v>
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13">
+        <f t="shared" si="0"/>
+        <v>0.6100000000000001</v>
       </c>
       <c r="F12" s="1">
         <v>7</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>1.65625</v>
+        <f t="shared" si="7"/>
+        <v>0.9375</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="2"/>
-        <v>1.671875</v>
+        <f t="shared" si="8"/>
+        <v>0.953125</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="3"/>
-        <v>1.6640625</v>
+        <f t="shared" si="1"/>
+        <v>0.9453125</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="4"/>
-        <v>-4.6701049804704908E-3</v>
+        <f t="shared" si="2"/>
+        <v>-1.7504224777221689E-2</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="5"/>
-        <v>0.11604640960693224</v>
+        <f t="shared" si="3"/>
+        <v>0.12214143260382126</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="6"/>
-        <v>5.5404782295225274E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.0970793772430634E-2</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="7"/>
-        <v>-2.5874614973881485E-4</v>
+        <f t="shared" si="5"/>
+        <v>-8.922042312660372E-4</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="8"/>
-        <v>5.5404782295225274E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.0970793772430634E-2</v>
       </c>
       <c r="O12" s="1" t="str">
         <f t="shared" si="9"/>
@@ -915,46 +934,47 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
-        <v>7</v>
+      <c r="B13" s="9">
+        <v>2</v>
       </c>
       <c r="C13" s="1">
-        <v>314.76</v>
+        <f t="shared" si="0"/>
+        <v>85.46</v>
       </c>
       <c r="F13" s="1">
         <v>8</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>1.65625</v>
+        <f t="shared" si="7"/>
+        <v>0.9375</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6640625</v>
+        <f t="shared" si="8"/>
+        <v>0.9453125</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="3"/>
-        <v>1.66015625</v>
+        <f t="shared" si="1"/>
+        <v>0.94140625</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="4"/>
-        <v>-4.6701049804704908E-3</v>
+        <f t="shared" si="2"/>
+        <v>-1.7504224777221689E-2</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="5"/>
-        <v>5.5404782295225274E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.0970793772430634E-2</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="6"/>
-        <v>2.5296662449835416E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.6400899609388953E-2</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="7"/>
-        <v>-1.1813806929625722E-4</v>
+        <f t="shared" si="5"/>
+        <v>-2.8708503331139164E-4</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="8"/>
-        <v>2.5296662449835416E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.6400899609388953E-2</v>
       </c>
       <c r="O13" s="1" t="str">
         <f t="shared" si="9"/>
@@ -963,45 +983,46 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1">
-        <v>471.93</v>
+        <f t="shared" si="0"/>
+        <v>695.07</v>
       </c>
       <c r="F14" s="1">
         <v>9</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
-        <v>1.65625</v>
+        <f t="shared" si="7"/>
+        <v>0.9375</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="2"/>
-        <v>1.66015625</v>
+        <f t="shared" si="8"/>
+        <v>0.94140625</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="3"/>
-        <v>1.658203125</v>
+        <f t="shared" si="1"/>
+        <v>0.939453125</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="4"/>
-        <v>-4.6701049804704908E-3</v>
+        <f t="shared" si="2"/>
+        <v>-1.7504224777221689E-2</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="5"/>
-        <v>2.5296662449835416E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.6400899609388953E-2</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="6"/>
-        <v>1.0295630469915551E-2</v>
+        <f t="shared" si="4"/>
+        <v>-6.341921599017919E-4</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="7"/>
-        <v>-4.8081675134636357E-5</v>
+        <f t="shared" si="5"/>
+        <v>1.1101042118872684E-5</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="8"/>
-        <v>1.0295630469915551E-2</v>
+        <f t="shared" si="6"/>
+        <v>6.341921599017919E-4</v>
       </c>
       <c r="O14" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1009,46 +1030,47 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
-        <v>9</v>
+      <c r="B15" s="9">
+        <v>4</v>
       </c>
       <c r="C15" s="1">
-        <v>673.74</v>
+        <f t="shared" si="0"/>
+        <v>2988.82</v>
       </c>
       <c r="F15" s="1">
         <v>10</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>1.65625</v>
+        <f t="shared" si="7"/>
+        <v>0.939453125</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="2"/>
-        <v>1.658203125</v>
+        <f t="shared" si="8"/>
+        <v>0.94140625</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="3"/>
-        <v>1.6572265625</v>
+        <f t="shared" si="1"/>
+        <v>0.9404296875</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="4"/>
-        <v>-4.6701049804704908E-3</v>
+        <f t="shared" si="2"/>
+        <v>-6.341921599017919E-4</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="5"/>
-        <v>1.0295630469915551E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.6400899609388953E-2</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="6"/>
-        <v>2.8083532769223041E-3</v>
+        <f t="shared" si="4"/>
+        <v>7.8626506918726413E-3</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="7"/>
-        <v>-1.3115304625475477E-5</v>
+        <f t="shared" si="5"/>
+        <v>-4.9864314248320285E-6</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="8"/>
-        <v>2.8083532769223041E-3</v>
+        <f t="shared" si="6"/>
+        <v>7.8626506918726413E-3</v>
       </c>
       <c r="O15" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1057,45 +1079,46 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
-        <v>925.77</v>
+        <f t="shared" si="0"/>
+        <v>9202.49</v>
       </c>
       <c r="F16" s="1">
         <v>11</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>1.65625</v>
+        <f t="shared" si="7"/>
+        <v>0.939453125</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6572265625</v>
+        <f t="shared" si="8"/>
+        <v>0.9404296875</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="3"/>
-        <v>1.65673828125</v>
+        <f t="shared" si="1"/>
+        <v>0.93994140625</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="4"/>
-        <v>-4.6701049804704908E-3</v>
+        <f t="shared" si="2"/>
+        <v>-6.341921599017919E-4</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="5"/>
-        <v>2.8083532769223041E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.8626506918726413E-3</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="6"/>
-        <v>-9.319778939262946E-4</v>
+        <f t="shared" si="4"/>
+        <v>3.609062349606118E-3</v>
       </c>
       <c r="M16" s="1">
-        <f t="shared" si="7"/>
-        <v>4.3524346041135869E-6</v>
+        <f t="shared" si="5"/>
+        <v>-2.2888390467169401E-6</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="8"/>
-        <v>9.319778939262946E-4</v>
+        <f t="shared" si="6"/>
+        <v>3.609062349606118E-3</v>
       </c>
       <c r="O16" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1107,45 +1130,45 @@
         <v>12</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="1"/>
-        <v>1.65673828125</v>
+        <f t="shared" si="7"/>
+        <v>0.939453125</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6572265625</v>
+        <f t="shared" si="8"/>
+        <v>0.93994140625</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="3"/>
-        <v>1.656982421875</v>
+        <f t="shared" si="1"/>
+        <v>0.939697265625</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="4"/>
-        <v>-9.319778939262946E-4</v>
+        <f t="shared" si="2"/>
+        <v>-6.341921599017919E-4</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="5"/>
-        <v>2.8083532769223041E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.609062349606118E-3</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" si="6"/>
-        <v>9.3791214035920945E-4</v>
+        <f t="shared" si="4"/>
+        <v>1.486144469938333E-3</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" si="7"/>
-        <v>-8.741133812598792E-7</v>
+        <f t="shared" si="5"/>
+        <v>-9.4250117131629511E-7</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="8"/>
-        <v>9.3791214035920945E-4</v>
+        <f t="shared" si="6"/>
+        <v>1.486144469938333E-3</v>
       </c>
       <c r="O17" s="1" t="str">
         <f t="shared" si="9"/>
         <v>CONTINUE</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="5" t="str">
         <f>_xlfn.CONCAT(" ", 10^-4)</f>
@@ -1155,40 +1178,40 @@
         <v>13</v>
       </c>
       <c r="G18" s="9">
-        <f t="shared" si="1"/>
-        <v>1.65673828125</v>
+        <f t="shared" si="7"/>
+        <v>0.939453125</v>
       </c>
       <c r="H18" s="9">
-        <f t="shared" si="2"/>
-        <v>1.656982421875</v>
-      </c>
-      <c r="I18" s="9">
-        <f t="shared" si="3"/>
-        <v>1.6568603515625</v>
-      </c>
-      <c r="J18" s="9">
-        <f t="shared" si="4"/>
-        <v>-9.319778939262946E-4</v>
-      </c>
-      <c r="K18" s="9">
-        <f t="shared" si="5"/>
-        <v>9.3791214035920945E-4</v>
-      </c>
-      <c r="L18" s="9">
-        <f t="shared" si="6"/>
-        <v>2.8982405080313356E-6</v>
-      </c>
-      <c r="M18" s="9">
-        <f t="shared" si="7"/>
-        <v>-2.7010960847669182E-9</v>
-      </c>
-      <c r="N18" s="9">
         <f t="shared" si="8"/>
-        <v>2.8982405080313356E-6</v>
+        <v>0.939697265625</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.9395751953125</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="2"/>
+        <v>-6.341921599017919E-4</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="3"/>
+        <v>1.486144469938333E-3</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="4"/>
+        <v>4.256536367470698E-4</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="5"/>
+        <v>-2.6994619925867691E-7</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="6"/>
+        <v>4.256536367470698E-4</v>
       </c>
       <c r="O18" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>STOP</v>
+        <v>CONTINUE</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
@@ -1196,36 +1219,36 @@
         <v>14</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="1"/>
-        <v>1.65673828125</v>
+        <f t="shared" si="7"/>
+        <v>0.939453125</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6568603515625</v>
+        <f t="shared" si="8"/>
+        <v>0.9395751953125</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="3"/>
-        <v>1.65679931640625</v>
+        <f t="shared" si="1"/>
+        <v>0.93951416015625</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="4"/>
-        <v>-9.319778939262946E-4</v>
+        <f t="shared" si="2"/>
+        <v>-6.341921599017919E-4</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="5"/>
-        <v>2.8982405080313356E-6</v>
+        <f t="shared" si="3"/>
+        <v>4.256536367470698E-4</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="6"/>
-        <v>-4.6455704675185672E-4</v>
+        <f t="shared" si="4"/>
+        <v>-1.0434987390461892E-4</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="7"/>
-        <v>4.3295689804041459E-7</v>
+        <f t="shared" si="5"/>
+        <v>6.6177871917049902E-8</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="8"/>
-        <v>4.6455704675185672E-4</v>
+        <f t="shared" si="6"/>
+        <v>1.0434987390461892E-4</v>
       </c>
       <c r="O19" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1237,40 +1260,245 @@
         <v>15</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="1"/>
-        <v>1.65679931640625</v>
+        <f t="shared" si="7"/>
+        <v>0.93951416015625</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6568603515625</v>
+        <f t="shared" si="8"/>
+        <v>0.9395751953125</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="3"/>
-        <v>1.656829833984375</v>
+        <f t="shared" si="1"/>
+        <v>0.939544677734375</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="4"/>
-        <v>-4.6455704675185672E-4</v>
+        <f t="shared" si="2"/>
+        <v>-1.0434987390461892E-4</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="5"/>
-        <v>2.8982405080313356E-6</v>
+        <f t="shared" si="3"/>
+        <v>4.256536367470698E-4</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="6"/>
-        <v>-2.3083370821286309E-4</v>
+        <f t="shared" si="4"/>
+        <v>1.6063172618463462E-4</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="7"/>
-        <v>1.0723542577814749E-7</v>
+        <f t="shared" si="5"/>
+        <v>-1.6761900372447894E-8</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="8"/>
-        <v>2.3083370821286309E-4</v>
+        <f t="shared" si="6"/>
+        <v>1.6063172618463462E-4</v>
       </c>
       <c r="O20" s="1" t="str">
         <f t="shared" si="9"/>
         <v>CONTINUE</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F21" s="14">
+        <v>16</v>
+      </c>
+      <c r="G21" s="14">
+        <f t="shared" ref="G21:G25" si="10">IF(M20&gt;0,I20,G20)</f>
+        <v>0.93951416015625</v>
+      </c>
+      <c r="H21" s="14">
+        <f t="shared" ref="H21:H25" si="11">IF(M20&lt;0,I20,H20)</f>
+        <v>0.939544677734375</v>
+      </c>
+      <c r="I21" s="14">
+        <f t="shared" si="1"/>
+        <v>0.9395294189453125</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="2"/>
+        <v>-1.0434987390461892E-4</v>
+      </c>
+      <c r="K21" s="14">
+        <f t="shared" si="3"/>
+        <v>1.6063172618463462E-4</v>
+      </c>
+      <c r="L21" s="14">
+        <f t="shared" si="4"/>
+        <v>2.8135887600200249E-5</v>
+      </c>
+      <c r="M21" s="14">
+        <f t="shared" si="5"/>
+        <v>-2.935976323275427E-9</v>
+      </c>
+      <c r="N21" s="14">
+        <f t="shared" si="6"/>
+        <v>2.8135887600200249E-5</v>
+      </c>
+      <c r="O21" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>STOP</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F22" s="14">
+        <v>17</v>
+      </c>
+      <c r="G22" s="14">
+        <f t="shared" si="10"/>
+        <v>0.93951416015625</v>
+      </c>
+      <c r="H22" s="14">
+        <f t="shared" si="11"/>
+        <v>0.9395294189453125</v>
+      </c>
+      <c r="I22" s="14">
+        <f t="shared" si="1"/>
+        <v>0.93952178955078125</v>
+      </c>
+      <c r="J22" s="14">
+        <f t="shared" si="2"/>
+        <v>-1.0434987390461892E-4</v>
+      </c>
+      <c r="K22" s="14">
+        <f t="shared" si="3"/>
+        <v>2.8135887600200249E-5</v>
+      </c>
+      <c r="L22" s="14">
+        <f t="shared" si="4"/>
+        <v>-3.8108252753632499E-5</v>
+      </c>
+      <c r="M22" s="14">
+        <f t="shared" si="5"/>
+        <v>3.9765913695668981E-9</v>
+      </c>
+      <c r="N22" s="14">
+        <f t="shared" si="6"/>
+        <v>3.8108252753632499E-5</v>
+      </c>
+      <c r="O22" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>STOP</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F23" s="14">
+        <v>18</v>
+      </c>
+      <c r="G23" s="14">
+        <f t="shared" si="10"/>
+        <v>0.93952178955078125</v>
+      </c>
+      <c r="H23" s="14">
+        <f t="shared" si="11"/>
+        <v>0.9395294189453125</v>
+      </c>
+      <c r="I23" s="14">
+        <f t="shared" si="1"/>
+        <v>0.93952560424804688</v>
+      </c>
+      <c r="J23" s="14">
+        <f t="shared" si="2"/>
+        <v>-3.8108252753632499E-5</v>
+      </c>
+      <c r="K23" s="14">
+        <f t="shared" si="3"/>
+        <v>2.8135887600200249E-5</v>
+      </c>
+      <c r="L23" s="14">
+        <f t="shared" si="4"/>
+        <v>-4.9864974809299412E-6</v>
+      </c>
+      <c r="M23" s="14">
+        <f t="shared" si="5"/>
+        <v>1.9002670635862996E-10</v>
+      </c>
+      <c r="N23" s="14">
+        <f t="shared" si="6"/>
+        <v>4.9864974809299412E-6</v>
+      </c>
+      <c r="O23" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>STOP</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F24" s="14">
+        <v>19</v>
+      </c>
+      <c r="G24" s="14">
+        <f t="shared" si="10"/>
+        <v>0.93952560424804688</v>
+      </c>
+      <c r="H24" s="14">
+        <f t="shared" si="11"/>
+        <v>0.9395294189453125</v>
+      </c>
+      <c r="I24" s="14">
+        <f t="shared" si="1"/>
+        <v>0.93952751159667969</v>
+      </c>
+      <c r="J24" s="14">
+        <f t="shared" si="2"/>
+        <v>-4.9864974809299412E-6</v>
+      </c>
+      <c r="K24" s="14">
+        <f t="shared" si="3"/>
+        <v>2.8135887600200249E-5</v>
+      </c>
+      <c r="L24" s="14">
+        <f t="shared" si="4"/>
+        <v>1.1574616332499232E-5</v>
+      </c>
+      <c r="M24" s="14">
+        <f t="shared" si="5"/>
+        <v>-5.7716795184737975E-11</v>
+      </c>
+      <c r="N24" s="14">
+        <f t="shared" si="6"/>
+        <v>1.1574616332499232E-5</v>
+      </c>
+      <c r="O24" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>STOP</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F25" s="14">
+        <v>20</v>
+      </c>
+      <c r="G25" s="14">
+        <f t="shared" si="10"/>
+        <v>0.93952560424804688</v>
+      </c>
+      <c r="H25" s="14">
+        <f t="shared" si="11"/>
+        <v>0.93952751159667969</v>
+      </c>
+      <c r="I25" s="14">
+        <f t="shared" si="1"/>
+        <v>0.93952655792236328</v>
+      </c>
+      <c r="J25" s="14">
+        <f t="shared" si="2"/>
+        <v>-4.9864974809299412E-6</v>
+      </c>
+      <c r="K25" s="14">
+        <f t="shared" si="3"/>
+        <v>1.1574616332499232E-5</v>
+      </c>
+      <c r="L25" s="14">
+        <f t="shared" si="4"/>
+        <v>3.2940397438618874E-6</v>
+      </c>
+      <c r="M25" s="14">
+        <f t="shared" si="5"/>
+        <v>-1.642572088485041E-11</v>
+      </c>
+      <c r="N25" s="14">
+        <f t="shared" si="6"/>
+        <v>3.2940397438618874E-6</v>
+      </c>
+      <c r="O25" s="14" t="str">
+        <f t="shared" si="9"/>
+        <v>STOP</v>
       </c>
     </row>
   </sheetData>

</xml_diff>